<commit_message>
explicacion de cada metodo comentada
</commit_message>
<xml_diff>
--- a/Book4.xlsx
+++ b/Book4.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/Documents/GitHub/M_ProgramacionAvanzada_Proyecto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{03DDDC4B-C66A-FF4F-9EA9-13567C86F59C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC40B1F2-E059-F548-BB70-FC0A8E2FD2B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="68800" windowHeight="28800" xr2:uid="{5069AB02-59F4-4940-84B5-537D71BA0C1A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25980" windowHeight="28800" xr2:uid="{5069AB02-59F4-4940-84B5-537D71BA0C1A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="29">
   <si>
     <t>Tamaño original</t>
   </si>
@@ -62,34 +62,76 @@
     <t>(25, 2,000,000)</t>
   </si>
   <si>
-    <t>(10, 324,342)</t>
-  </si>
-  <si>
     <t>Serial</t>
   </si>
   <si>
     <t>Col[0] == 1</t>
   </si>
   <si>
-    <t>(20, 1,058,818)</t>
-  </si>
-  <si>
     <t>Col[10] &lt;= 0.3</t>
   </si>
   <si>
-    <t>(12, 18,941)</t>
-  </si>
-  <si>
     <t>Col[20] &gt;=1</t>
   </si>
   <si>
-    <t>(6, 425,850)</t>
+    <t>Col[11]&gt;0.1</t>
+  </si>
+  <si>
+    <t>Col[0] == 0</t>
+  </si>
+  <si>
+    <t>Sin filtrado</t>
+  </si>
+  <si>
+    <t>Col[15] &lt; 0.8</t>
+  </si>
+  <si>
+    <t>Col[2] &lt;= 0.3</t>
+  </si>
+  <si>
+    <t>Col[22] &gt; 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speedup </t>
+  </si>
+  <si>
+    <t>(24: 551,445)</t>
+  </si>
+  <si>
+    <t>(10: 324,342)</t>
+  </si>
+  <si>
+    <t>(20: 1,058,818)</t>
+  </si>
+  <si>
+    <t>(12: 18,941)</t>
+  </si>
+  <si>
+    <t>(6: 425,850)</t>
+  </si>
+  <si>
+    <t>(16: 924,453)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (21: 941,182)</t>
+  </si>
+  <si>
+    <t>(21: 2000,000)</t>
+  </si>
+  <si>
+    <t>(17: 5,425)</t>
+  </si>
+  <si>
+    <t>(6: 1,213,483)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.0"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -113,7 +155,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -121,18 +163,287 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="10">
+    <dxf>
+      <numFmt numFmtId="168" formatCode="0.0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -143,6 +454,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{56CA4016-867B-8347-A270-B3BD799F3BC9}" name="Table1" displayName="Table1" ref="A2:F22" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="8" tableBorderDxfId="9" totalsRowBorderDxfId="7">
+  <autoFilter ref="A2:F22" xr:uid="{56CA4016-867B-8347-A270-B3BD799F3BC9}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{E645A7BE-45CE-9443-9BD0-B36165375F0C}" name="Secuencial/Concurrente" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{DA64B0D3-7E95-8C40-909D-3838098BCC30}" name="Tamaño original" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{929F3527-EE0F-A740-BBF1-AF03640F0775}" name="Tamaño filtrado" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{1A9D8512-79DA-D94E-80D8-ED84191061D2}" name="Criterio de filtrado" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{EDC5FDDA-2E6C-B844-AF11-727E75F1DE88}" name="Tiempo de ejecución (s)" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{3C379226-5C55-F54E-B4B4-5BA8EAD203D7}" name="Speedup " dataDxfId="0">
+      <calculatedColumnFormula>E4/Table1[[#This Row],[Tiempo de ejecución (s)]]</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -442,176 +770,437 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF30DE69-84A8-C44E-B374-4CF0F9D68B9C}">
-  <dimension ref="A2:E10"/>
+  <dimension ref="A2:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.83203125" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18.5" customWidth="1"/>
+    <col min="5" max="5" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="F2" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="4">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="F3" s="11">
+        <f>E4/Table1[[#This Row],[Tiempo de ejecución (s)]]</f>
+        <v>2.2173913043478262</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E3">
-        <v>4.5999999999999996</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="E4" s="4">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="F4" s="12"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="E5" s="4">
+        <v>4.3</v>
+      </c>
+      <c r="F5" s="12">
+        <f>E6/Table1[[#This Row],[Tiempo de ejecución (s)]]</f>
+        <v>2.441860465116279</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4">
-        <v>10.199999999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="4">
+        <v>10.5</v>
+      </c>
+      <c r="F6" s="12"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="4">
+        <v>2.9</v>
+      </c>
+      <c r="F7" s="12">
+        <f>E8/Table1[[#This Row],[Tiempo de ejecución (s)]]</f>
+        <v>3.3793103448275867</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="4">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="F8" s="12"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E9" s="4">
+        <v>3.4</v>
+      </c>
+      <c r="F9" s="12">
+        <f>E10/Table1[[#This Row],[Tiempo de ejecución (s)]]</f>
+        <v>2.9411764705882355</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="10">
         <v>10</v>
       </c>
-      <c r="E5">
-        <v>4.3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6">
-        <v>10.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="F10" s="12"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="4">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="F11" s="12">
+        <f>E12/Table1[[#This Row],[Tiempo de ejecución (s)]]</f>
+        <v>2.6274509803921573</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="4">
+        <v>13.4</v>
+      </c>
+      <c r="F12" s="12"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E13" s="4">
+        <v>4.7</v>
+      </c>
+      <c r="F13" s="12">
+        <f>E14/Table1[[#This Row],[Tiempo de ejecución (s)]]</f>
+        <v>2.5531914893617018</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="4">
         <v>12</v>
       </c>
-      <c r="E7">
-        <v>2.9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="F14" s="12"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8">
-        <v>9.8000000000000007</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="B15" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="4">
+        <v>5.8</v>
+      </c>
+      <c r="F15" s="12">
+        <f>E16/Table1[[#This Row],[Tiempo de ejecución (s)]]</f>
+        <v>2.603448275862069</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="4">
+        <v>15.1</v>
+      </c>
+      <c r="F16" s="12"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9">
-        <v>3.4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="E17" s="4">
+        <v>5.4</v>
+      </c>
+      <c r="F17" s="12">
+        <f>E18/Table1[[#This Row],[Tiempo de ejecución (s)]]</f>
+        <v>2.3888888888888888</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="10">
+        <v>12.9</v>
+      </c>
+      <c r="F18" s="12"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10">
-        <v>10</v>
-      </c>
+      <c r="B19" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="4">
+        <v>5</v>
+      </c>
+      <c r="F19" s="12">
+        <f>E20/Table1[[#This Row],[Tiempo de ejecución (s)]]</f>
+        <v>2.2600000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="10">
+        <v>11.3</v>
+      </c>
+      <c r="F20" s="12"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="4">
+        <v>4.2</v>
+      </c>
+      <c r="F21" s="12">
+        <f>E22/Table1[[#This Row],[Tiempo de ejecución (s)]]</f>
+        <v>2.7142857142857144</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="10">
+        <v>11.4</v>
+      </c>
+      <c r="F22" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modificacion a estructura de carpetas
</commit_message>
<xml_diff>
--- a/Book4.xlsx
+++ b/Book4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/Documents/GitHub/M_ProgramacionAvanzada_Proyecto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC40B1F2-E059-F548-BB70-FC0A8E2FD2B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5DA6EA3-79D5-5541-97C6-BDA3A040E6C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25980" windowHeight="28800" xr2:uid="{5069AB02-59F4-4940-84B5-537D71BA0C1A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="68800" windowHeight="28300" xr2:uid="{5069AB02-59F4-4940-84B5-537D71BA0C1A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -454,6 +454,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>201705</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>309282</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>170888</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8483E337-C082-B1A8-A37A-63AB8AB24E30}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14552706" y="2622176"/>
+          <a:ext cx="7772400" cy="3801594"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -773,7 +822,7 @@
   <dimension ref="A2:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:F23"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1199,8 +1248,9 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>